<commit_message>
Riesecuzione test per problematiche tecniche
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#PANTAREIINFORMATICASRLXX/PANTAREIINFORMATICASRL/CASSIOPEA/1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#PANTAREIINFORMATICASRLXX/PANTAREIINFORMATICASRL/CASSIOPEA/1.0.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1invii\1Clienti\fse\Accreditamento\publish\A1#111#PANTAREIINFORMATICASRLXX\PANTAREIINFORMATICASRL\CASSIOPEA\1.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8347289-774B-40DA-B3A7-FAE193BDDCA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81F7E3C-6ED0-4805-AD86-F6918EBE8CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -1707,15 +1707,6 @@
     <t>L'operazione viene eseguita manualmente dall'operatore</t>
   </si>
   <si>
-    <t>2025-04-07T14:57:05Z</t>
-  </si>
-  <si>
-    <t>19c0eb662b5c64f7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.f7bc2d9bf5adb3259b07e198737501f4a9163f4cdc35be22828f08bc4ba0d2d6.c83b3bb22a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>PANTAREIINFORMATICASRL</t>
   </si>
   <si>
@@ -1726,6 +1717,15 @@
   </si>
   <si>
     <t>subject_application_version:1.0.0</t>
+  </si>
+  <si>
+    <t>2025-05-07T15:21:38Z</t>
+  </si>
+  <si>
+    <t>42faa74815ae93917c5975dc897dfca2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.f7bc2d9bf5adb3259b07e198737501f4a9163f4cdc35be22828f08bc4ba0d2d6.5a1b7ff8dc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3811,11 +3811,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:W756"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E28" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
+      <selection pane="bottomRight" activeCell="I172" sqref="I172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3862,7 +3862,7 @@
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="50" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D2" s="49"/>
       <c r="F2" s="6"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="B3" s="52"/>
       <c r="C3" s="57" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D3" s="49"/>
       <c r="F3" s="6"/>
@@ -3916,7 +3916,7 @@
       <c r="A4" s="53"/>
       <c r="B4" s="54"/>
       <c r="C4" s="57" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="4"/>
@@ -3943,7 +3943,7 @@
       <c r="A5" s="55"/>
       <c r="B5" s="56"/>
       <c r="C5" s="57" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D5" s="49"/>
       <c r="F5" s="6"/>
@@ -10193,16 +10193,16 @@
         <v>383</v>
       </c>
       <c r="F172" s="33">
-        <v>45754</v>
+        <v>45784</v>
       </c>
       <c r="G172" s="33" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="H172" s="33" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="I172" s="39" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="J172" s="29" t="s">
         <v>66</v>
@@ -17341,6 +17341,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17598,42 +17619,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17656,9 +17645,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
test con checklist v.8.2.5
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#PANTAREIINFORMATICASRLXX/PANTAREIINFORMATICASRL/CASSIOPEA/1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#PANTAREIINFORMATICASRLXX/PANTAREIINFORMATICASRL/CASSIOPEA/1.0.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1invii\1Clienti\fse\Accreditamento\publish\A1#111#PANTAREIINFORMATICASRLXX\PANTAREIINFORMATICASRL\CASSIOPEA\1.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81F7E3C-6ED0-4805-AD86-F6918EBE8CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5085005A-DFAE-46CB-A2D6-22BC26AF4B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -1719,13 +1719,13 @@
     <t>subject_application_version:1.0.0</t>
   </si>
   <si>
-    <t>2025-05-07T15:21:38Z</t>
-  </si>
-  <si>
-    <t>42faa74815ae93917c5975dc897dfca2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.f7bc2d9bf5adb3259b07e198737501f4a9163f4cdc35be22828f08bc4ba0d2d6.5a1b7ff8dc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-05-08T15:17:15Z</t>
+  </si>
+  <si>
+    <t>71ddc1ac3b9dc68a146e1656987ecc6e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.f7bc2d9bf5adb3259b07e198737501f4a9163f4cdc35be22828f08bc4ba0d2d6.f47f34395f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3811,8 +3811,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:W756"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="D52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="I172" sqref="I172"/>
@@ -7401,7 +7401,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="31">
         <v>127</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="31">
         <v>128</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="31">
         <v>129</v>
       </c>
@@ -7512,7 +7512,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="31">
         <v>130</v>
       </c>
@@ -7549,7 +7549,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="31">
         <v>131</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="31">
         <v>132</v>
       </c>
@@ -7623,7 +7623,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="31">
         <v>133</v>
       </c>
@@ -7660,7 +7660,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="31">
         <v>134</v>
       </c>
@@ -7697,7 +7697,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="31">
         <v>135</v>
       </c>
@@ -7734,7 +7734,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="31">
         <v>136</v>
       </c>
@@ -7771,7 +7771,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="107" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="31">
         <v>137</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="31">
         <v>138</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="109" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="31">
         <v>139</v>
       </c>
@@ -7882,7 +7882,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="31">
         <v>140</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="111" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="31">
         <v>141</v>
       </c>
@@ -7956,7 +7956,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="31">
         <v>142</v>
       </c>
@@ -7993,7 +7993,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="113" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="31">
         <v>143</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="114" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="31">
         <v>144</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="115" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="31">
         <v>145</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="31">
         <v>146</v>
       </c>
@@ -10193,7 +10193,7 @@
         <v>383</v>
       </c>
       <c r="F172" s="33">
-        <v>45784</v>
+        <v>45785</v>
       </c>
       <c r="G172" s="33" t="s">
         <v>440</v>
@@ -10634,7 +10634,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="31">
         <v>463</v>
       </c>
@@ -17341,27 +17341,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17619,10 +17598,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17645,20 +17656,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
correzione report-checklist compilazione v.8.2.5
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#PANTAREIINFORMATICASRLXX/PANTAREIINFORMATICASRL/CASSIOPEA/1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#PANTAREIINFORMATICASRLXX/PANTAREIINFORMATICASRL/CASSIOPEA/1.0.0/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1invii\1Clienti\fse\Accreditamento\git-rsa-rad\it-fse-accreditamento-rad-rsa\GATEWAY\A1#111#PANTAREIINFORMATICASRLXX\PANTAREIINFORMATICASRL\CASSIOPEA\1.0.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1invii\1Clienti\fse\Accreditamento\publish\A1#111#PANTAREIINFORMATICASRLXX\PANTAREIINFORMATICASRL\CASSIOPEA\1.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B63CE4-0619-4F91-959D-96A32EE83EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6D8BDA-4502-4C5D-A9D5-5CD44C1FA0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="446">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1723,19 +1723,19 @@
     <t>subject_application_version:1.0.0</t>
   </si>
   <si>
+    <t>2025-05-12T10:02:46Z</t>
+  </si>
+  <si>
+    <t>d59fdd1d8bc25a1ef66bb854d13384e8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.f7bc2d9bf5adb3259b07e198737501f4a9163f4cdc35be22828f08bc4ba0d2d6.7f7356e1de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
     <t>Mostra un messaggio di errore all'operatore riportando la risposta fornita dal gateway</t>
   </si>
   <si>
     <t>L'operazione viene eseguita manualmente dall'operatore</t>
-  </si>
-  <si>
-    <t>2025-05-12T10:02:46Z</t>
-  </si>
-  <si>
-    <t>d59fdd1d8bc25a1ef66bb854d13384e8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.f7bc2d9bf5adb3259b07e198737501f4a9163f4cdc35be22828f08bc4ba0d2d6.7f7356e1de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3799,11 +3799,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:W755"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H171" sqref="H171"/>
+      <selection pane="bottomRight" activeCell="K187" sqref="K187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4187,7 +4187,9 @@
       <c r="J12" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K12" s="38"/>
+      <c r="K12" s="38" t="s">
+        <v>239</v>
+      </c>
       <c r="L12" s="38"/>
       <c r="M12" s="38"/>
       <c r="N12" s="38"/>
@@ -4485,7 +4487,9 @@
       <c r="J20" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K20" s="38"/>
+      <c r="K20" s="38" t="s">
+        <v>239</v>
+      </c>
       <c r="L20" s="38"/>
       <c r="M20" s="38"/>
       <c r="N20" s="38"/>
@@ -4794,7 +4798,7 @@
         <v>64</v>
       </c>
       <c r="O28" s="38" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="P28" s="38" t="s">
         <v>64</v>
@@ -4806,7 +4810,7 @@
         <v>64</v>
       </c>
       <c r="S28" s="38" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="T28" s="38"/>
       <c r="U28" s="39" t="s">
@@ -5407,7 +5411,9 @@
       <c r="J44" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K44" s="38"/>
+      <c r="K44" s="38" t="s">
+        <v>242</v>
+      </c>
       <c r="L44" s="38"/>
       <c r="M44" s="38"/>
       <c r="N44" s="38"/>
@@ -5446,7 +5452,9 @@
       <c r="J45" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K45" s="38"/>
+      <c r="K45" s="38" t="s">
+        <v>242</v>
+      </c>
       <c r="L45" s="38"/>
       <c r="M45" s="38"/>
       <c r="N45" s="38"/>
@@ -5485,7 +5493,9 @@
       <c r="J46" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K46" s="38"/>
+      <c r="K46" s="38" t="s">
+        <v>242</v>
+      </c>
       <c r="L46" s="38"/>
       <c r="M46" s="38"/>
       <c r="N46" s="38"/>
@@ -5524,7 +5534,9 @@
       <c r="J47" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K47" s="38"/>
+      <c r="K47" s="38" t="s">
+        <v>242</v>
+      </c>
       <c r="L47" s="38"/>
       <c r="M47" s="38"/>
       <c r="N47" s="38"/>
@@ -5563,7 +5575,9 @@
       <c r="J48" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K48" s="38"/>
+      <c r="K48" s="38" t="s">
+        <v>242</v>
+      </c>
       <c r="L48" s="38"/>
       <c r="M48" s="38"/>
       <c r="N48" s="38"/>
@@ -5602,7 +5616,9 @@
       <c r="J49" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K49" s="38"/>
+      <c r="K49" s="38" t="s">
+        <v>242</v>
+      </c>
       <c r="L49" s="38"/>
       <c r="M49" s="38"/>
       <c r="N49" s="38"/>
@@ -5641,7 +5657,9 @@
       <c r="J50" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K50" s="38"/>
+      <c r="K50" s="38" t="s">
+        <v>242</v>
+      </c>
       <c r="L50" s="38"/>
       <c r="M50" s="38"/>
       <c r="N50" s="38"/>
@@ -5680,7 +5698,9 @@
       <c r="J51" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K51" s="38"/>
+      <c r="K51" s="38" t="s">
+        <v>242</v>
+      </c>
       <c r="L51" s="38"/>
       <c r="M51" s="38"/>
       <c r="N51" s="38"/>
@@ -5719,7 +5739,9 @@
       <c r="J52" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K52" s="38"/>
+      <c r="K52" s="38" t="s">
+        <v>242</v>
+      </c>
       <c r="L52" s="38"/>
       <c r="M52" s="38"/>
       <c r="N52" s="38"/>
@@ -5758,7 +5780,9 @@
       <c r="J53" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K53" s="38"/>
+      <c r="K53" s="38" t="s">
+        <v>242</v>
+      </c>
       <c r="L53" s="38"/>
       <c r="M53" s="38"/>
       <c r="N53" s="38"/>
@@ -10123,13 +10147,13 @@
         <v>45789</v>
       </c>
       <c r="G171" s="37" t="s">
+        <v>441</v>
+      </c>
+      <c r="H171" s="37" t="s">
+        <v>442</v>
+      </c>
+      <c r="I171" s="42" t="s">
         <v>443</v>
-      </c>
-      <c r="H171" s="37" t="s">
-        <v>444</v>
-      </c>
-      <c r="I171" s="42" t="s">
-        <v>445</v>
       </c>
       <c r="J171" s="38" t="s">
         <v>64</v>
@@ -10173,7 +10197,9 @@
       <c r="J172" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K172" s="38"/>
+      <c r="K172" s="38" t="s">
+        <v>237</v>
+      </c>
       <c r="L172" s="38"/>
       <c r="M172" s="38"/>
       <c r="N172" s="38"/>
@@ -10730,7 +10756,9 @@
       <c r="J187" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K187" s="38"/>
+      <c r="K187" s="38" t="s">
+        <v>237</v>
+      </c>
       <c r="L187" s="35"/>
       <c r="M187" s="38"/>
       <c r="N187" s="38"/>
@@ -17298,6 +17326,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
@@ -17309,7 +17346,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17567,16 +17604,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -17593,7 +17629,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17610,12 +17646,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>